<commit_message>
finished the dataframe joining
</commit_message>
<xml_diff>
--- a/matchIndex.xlsx
+++ b/matchIndex.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -477,7 +477,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
@@ -507,7 +507,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9">
@@ -567,7 +567,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -597,7 +597,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12">
@@ -627,7 +627,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14">
@@ -642,7 +642,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -684,7 +684,7 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17">
@@ -699,7 +699,7 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>2</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="18">
@@ -714,7 +714,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19">
@@ -729,7 +729,7 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -744,7 +744,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>2</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="21">
@@ -786,7 +786,7 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -832,7 +832,7 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -847,7 +847,7 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26">
@@ -862,7 +862,7 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -891,7 +891,7 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28">
@@ -906,7 +906,7 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>3</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="29">
@@ -921,7 +921,7 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30">
@@ -936,7 +936,7 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31">
@@ -951,7 +951,7 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32">
@@ -966,7 +966,7 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -996,7 +996,7 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35">
@@ -1026,7 +1026,7 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>0</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="37">
@@ -1041,7 +1041,7 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38">
@@ -1071,7 +1071,7 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>1</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="40">
@@ -1088,7 +1088,7 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41">
@@ -1108,7 +1108,7 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>1</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="42">
@@ -1123,7 +1123,7 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>4</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="43">
@@ -1166,7 +1166,7 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="45">
@@ -1181,7 +1181,7 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46">
@@ -1196,7 +1196,7 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47">
@@ -1211,7 +1211,7 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>4</v>
+        <v>-5</v>
       </c>
     </row>
     <row r="48">
@@ -1226,7 +1226,7 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>7</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="49">
@@ -1241,7 +1241,7 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="50">
@@ -1256,7 +1256,7 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>7</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="51">
@@ -1271,7 +1271,7 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>9</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="52">
@@ -1292,7 +1292,7 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="53">
@@ -1338,7 +1338,7 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56">
@@ -1353,7 +1353,7 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="57">
@@ -1368,7 +1368,7 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58">
@@ -1383,7 +1383,7 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="59">
@@ -1405,7 +1405,7 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60">
@@ -1420,7 +1420,7 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>4</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="61">
@@ -1435,7 +1435,7 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>6</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="62">
@@ -1450,7 +1450,7 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>3</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="63">
@@ -1465,7 +1465,7 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64">
@@ -1515,7 +1515,7 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67">
@@ -1560,7 +1560,7 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="70">
@@ -1575,7 +1575,7 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="71">
@@ -1590,7 +1590,7 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72">
@@ -1609,7 +1609,7 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73">
@@ -1647,7 +1647,7 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75">
@@ -1668,7 +1668,7 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="76">
@@ -1683,7 +1683,7 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>3</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="77">
@@ -1702,7 +1702,7 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="78">
@@ -1717,7 +1717,7 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79">
@@ -1732,7 +1732,7 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>3</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="80">
@@ -1747,7 +1747,7 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81">
@@ -1762,7 +1762,7 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="82">
@@ -1777,7 +1777,7 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83">
@@ -1795,7 +1795,7 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="84">
@@ -1824,7 +1824,7 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85">
@@ -1854,7 +1854,7 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="87">
@@ -1869,7 +1869,7 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="88">
@@ -1897,7 +1897,7 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89">
@@ -1912,7 +1912,7 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="90">
@@ -1927,7 +1927,7 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>2</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="91">
@@ -1942,7 +1942,7 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>1</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="92">
@@ -1957,7 +1957,7 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>3</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="93">
@@ -1972,7 +1972,7 @@
         </is>
       </c>
       <c r="C93" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="94">
@@ -1987,7 +1987,7 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="95">
@@ -2002,7 +2002,7 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="96">
@@ -2017,7 +2017,7 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97">
@@ -2047,7 +2047,7 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="99">
@@ -2062,7 +2062,7 @@
         </is>
       </c>
       <c r="C99" t="n">
-        <v>2</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="100">
@@ -2077,7 +2077,7 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>0</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="101">
@@ -2112,7 +2112,7 @@
         </is>
       </c>
       <c r="C102" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="103">
@@ -2127,7 +2127,7 @@
         </is>
       </c>
       <c r="C103" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="104">
@@ -2147,7 +2147,7 @@
         </is>
       </c>
       <c r="C104" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="105">
@@ -2167,7 +2167,7 @@
         </is>
       </c>
       <c r="C105" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="106">
@@ -2182,7 +2182,7 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="107">
@@ -2197,7 +2197,7 @@
         </is>
       </c>
       <c r="C107" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="108">
@@ -2224,7 +2224,7 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="109">
@@ -2239,7 +2239,7 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="110">
@@ -2259,7 +2259,7 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>4</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="111">
@@ -2274,7 +2274,7 @@
         </is>
       </c>
       <c r="C111" t="n">
-        <v>1</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="112">
@@ -2304,7 +2304,7 @@
         </is>
       </c>
       <c r="C113" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="114">
@@ -2319,7 +2319,7 @@
         </is>
       </c>
       <c r="C114" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="115">
@@ -2334,7 +2334,7 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>3</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="116">
@@ -2355,7 +2355,7 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="117">
@@ -2385,7 +2385,7 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="119">
@@ -2400,7 +2400,7 @@
         </is>
       </c>
       <c r="C119" t="n">
-        <v>2</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="120">
@@ -2415,7 +2415,7 @@
         </is>
       </c>
       <c r="C120" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="121">
@@ -2430,7 +2430,7 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="122">
@@ -2445,7 +2445,7 @@
         </is>
       </c>
       <c r="C122" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="123">
@@ -2464,7 +2464,7 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>6</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="124">
@@ -2489,7 +2489,7 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="125">
@@ -2504,7 +2504,7 @@
         </is>
       </c>
       <c r="C125" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="126">
@@ -2519,7 +2519,7 @@
         </is>
       </c>
       <c r="C126" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="127">
@@ -2534,7 +2534,7 @@
         </is>
       </c>
       <c r="C127" t="n">
-        <v>3</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="128">
@@ -2549,7 +2549,7 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>1</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="129">
@@ -2564,7 +2564,7 @@
         </is>
       </c>
       <c r="C129" t="n">
-        <v>0</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="130">
@@ -2579,7 +2579,7 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="131">
@@ -2594,7 +2594,7 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="132">
@@ -2617,7 +2617,7 @@
         </is>
       </c>
       <c r="C132" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="133">
@@ -2643,7 +2643,7 @@
         </is>
       </c>
       <c r="C133" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="134">
@@ -2669,7 +2669,7 @@
         </is>
       </c>
       <c r="C134" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="135">
@@ -2695,7 +2695,7 @@
         </is>
       </c>
       <c r="C135" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="136">
@@ -2721,7 +2721,7 @@
         </is>
       </c>
       <c r="C136" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="137">
@@ -2747,7 +2747,7 @@
         </is>
       </c>
       <c r="C137" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="138">
@@ -2773,7 +2773,7 @@
         </is>
       </c>
       <c r="C138" t="n">
-        <v>2</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="139">
@@ -2799,7 +2799,7 @@
         </is>
       </c>
       <c r="C139" t="n">
-        <v>2</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="140">
@@ -2825,7 +2825,7 @@
         </is>
       </c>
       <c r="C140" t="n">
-        <v>2</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="141">
@@ -2851,7 +2851,7 @@
         </is>
       </c>
       <c r="C141" t="n">
-        <v>2</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="142">
@@ -2875,7 +2875,7 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="143">
@@ -2944,7 +2944,7 @@
         </is>
       </c>
       <c r="C145" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="146">
@@ -2987,7 +2987,7 @@
         </is>
       </c>
       <c r="C146" t="n">
-        <v>7</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="147">
@@ -3017,7 +3017,7 @@
         </is>
       </c>
       <c r="C148" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="149">
@@ -3032,7 +3032,7 @@
         </is>
       </c>
       <c r="C149" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="150">
@@ -3064,7 +3064,7 @@
         </is>
       </c>
       <c r="C151" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="152">
@@ -3079,7 +3079,7 @@
         </is>
       </c>
       <c r="C152" t="n">
-        <v>3</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="153">
@@ -3094,7 +3094,7 @@
         </is>
       </c>
       <c r="C153" t="n">
-        <v>3</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="154">
@@ -3109,7 +3109,7 @@
         </is>
       </c>
       <c r="C154" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="155">
@@ -3124,7 +3124,7 @@
         </is>
       </c>
       <c r="C155" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="156">
@@ -3139,7 +3139,7 @@
         </is>
       </c>
       <c r="C156" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="157">
@@ -3169,7 +3169,7 @@
         </is>
       </c>
       <c r="C158" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="159">
@@ -3224,7 +3224,7 @@
         </is>
       </c>
       <c r="C161" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="162">
@@ -3243,7 +3243,7 @@
         </is>
       </c>
       <c r="C162" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="163">
@@ -3258,7 +3258,7 @@
         </is>
       </c>
       <c r="C163" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="164">
@@ -3288,7 +3288,7 @@
         </is>
       </c>
       <c r="C165" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="166">
@@ -3303,7 +3303,7 @@
         </is>
       </c>
       <c r="C166" t="n">
-        <v>4</v>
+        <v>-5</v>
       </c>
     </row>
     <row r="167">
@@ -3333,7 +3333,7 @@
         </is>
       </c>
       <c r="C168" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="169">
@@ -3363,7 +3363,7 @@
         </is>
       </c>
       <c r="C170" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="171">
@@ -3378,7 +3378,7 @@
         </is>
       </c>
       <c r="C171" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="172">
@@ -3393,7 +3393,7 @@
         </is>
       </c>
       <c r="C172" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="173">
@@ -3408,7 +3408,7 @@
         </is>
       </c>
       <c r="C173" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="174">
@@ -3423,7 +3423,7 @@
         </is>
       </c>
       <c r="C174" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="175">
@@ -3453,7 +3453,7 @@
         </is>
       </c>
       <c r="C176" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="177">
@@ -3468,7 +3468,7 @@
         </is>
       </c>
       <c r="C177" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="178">
@@ -3484,7 +3484,7 @@
         </is>
       </c>
       <c r="C178" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="179">
@@ -3509,7 +3509,7 @@
         </is>
       </c>
       <c r="C179" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="180">
@@ -3539,7 +3539,7 @@
         </is>
       </c>
       <c r="C181" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="182">
@@ -3554,7 +3554,7 @@
         </is>
       </c>
       <c r="C182" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="183">
@@ -3577,7 +3577,7 @@
         </is>
       </c>
       <c r="C183" t="n">
-        <v>1</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="184">
@@ -3593,7 +3593,7 @@
         </is>
       </c>
       <c r="C184" t="n">
-        <v>3</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="185">
@@ -3620,7 +3620,7 @@
         </is>
       </c>
       <c r="C185" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="186">
@@ -3635,7 +3635,7 @@
         </is>
       </c>
       <c r="C186" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="187">
@@ -3674,7 +3674,7 @@
         </is>
       </c>
       <c r="C188" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="189">
@@ -3730,7 +3730,7 @@
         </is>
       </c>
       <c r="C191" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="192">
@@ -3750,7 +3750,7 @@
         </is>
       </c>
       <c r="C192" t="n">
-        <v>3</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="193">
@@ -3765,7 +3765,7 @@
         </is>
       </c>
       <c r="C193" t="n">
-        <v>7</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="194">
@@ -3780,7 +3780,7 @@
         </is>
       </c>
       <c r="C194" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="195">
@@ -3795,7 +3795,7 @@
         </is>
       </c>
       <c r="C195" t="n">
-        <v>2</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="196">
@@ -3833,7 +3833,7 @@
         </is>
       </c>
       <c r="C197" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="198">
@@ -3848,7 +3848,7 @@
         </is>
       </c>
       <c r="C198" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="199">
@@ -3863,7 +3863,7 @@
         </is>
       </c>
       <c r="C199" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="200">
@@ -3897,7 +3897,7 @@
         </is>
       </c>
       <c r="C201" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="202">
@@ -3912,7 +3912,7 @@
         </is>
       </c>
       <c r="C202" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="203">
@@ -3927,7 +3927,7 @@
         </is>
       </c>
       <c r="C203" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="204">
@@ -3942,7 +3942,7 @@
         </is>
       </c>
       <c r="C204" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="205">
@@ -3961,7 +3961,7 @@
         </is>
       </c>
       <c r="C205" t="n">
-        <v>4</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="206">
@@ -3976,7 +3976,7 @@
         </is>
       </c>
       <c r="C206" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="207">
@@ -3991,7 +3991,7 @@
         </is>
       </c>
       <c r="C207" t="n">
-        <v>2</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="208">
@@ -4015,7 +4015,7 @@
         </is>
       </c>
       <c r="C208" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="209">
@@ -4039,7 +4039,7 @@
         </is>
       </c>
       <c r="C209" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="210">
@@ -4057,7 +4057,7 @@
         </is>
       </c>
       <c r="C210" t="n">
-        <v>2</v>
+        <v>-1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>